<commit_message>
Modified arrangement of buttons on GUI. Now users can preview a task set they manually enter. They also have the ability to feed an excel sheet to the input to either schedule task sets via RMS, EDF, and get a sheet with both for each task set from the given input file. The outputted file now lists if the task set can or can not be scheduled based on the algorithm, prints the task set next to output and shows what the task set will look like when it is scheduled. Also a README was added to give better directions on how to use the application.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zango\PycharmProjects\pySchedulingGUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C815CCDE-8CB8-42E0-B6D6-2567DF240F52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D372AF2-0EDE-471C-8E30-4F7E25A68CCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6315" yWindow="4680" windowWidth="21600" windowHeight="11385" xr2:uid="{5BF990A5-4107-4CFF-90E1-2DA3DD86FD5B}"/>
   </bookViews>
@@ -34,24 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>3 4 7</t>
-  </si>
-  <si>
-    <t>1 2 8</t>
-  </si>
-  <si>
-    <t>1 2 3</t>
-  </si>
-  <si>
-    <t>4 5 6</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>2 2 5</t>
   </si>
   <si>
     <t>3 5 7</t>
+  </si>
+  <si>
+    <t>1 5 10</t>
   </si>
 </sst>
 </file>
@@ -403,36 +394,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2BEE62F-AEC1-4644-997E-8FE161DE8E0C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimized code a little bit by removing unnecessary print statements when printing to excel. Added coloring of cells for excel for better visual representation of results sheet.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zango\PycharmProjects\pySchedulingGUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D372AF2-0EDE-471C-8E30-4F7E25A68CCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15CA8AC-133F-473A-A041-CB48D8A4A0F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6315" yWindow="4680" windowWidth="21600" windowHeight="11385" xr2:uid="{5BF990A5-4107-4CFF-90E1-2DA3DD86FD5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5BF990A5-4107-4CFF-90E1-2DA3DD86FD5B}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>2 2 5</t>
+    <t>2 5 5</t>
   </si>
   <si>
-    <t>3 5 7</t>
-  </si>
-  <si>
-    <t>1 5 10</t>
+    <t>3 7 7</t>
   </si>
 </sst>
 </file>
@@ -394,24 +391,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2BEE62F-AEC1-4644-997E-8FE161DE8E0C}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>